<commit_message>
EPBDS-11364 External return doesn't match to the return column if parameters from Action and Condition are used and implicit case Integer-> Double is used
</commit_message>
<xml_diff>
--- a/STUDIO/org.openl.rules.test/test-resources/functionality/EPBDS-11364_SmartRules_ExternalReturnsMatch.xlsx
+++ b/STUDIO/org.openl.rules.test/test-resources/functionality/EPBDS-11364_SmartRules_ExternalReturnsMatch.xlsx
@@ -3,21 +3,21 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23901"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <mc:AlternateContent>
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mkama\.openl\user-workspace\DEFAULT\externalActionMatch(1)\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mkama\.openl\user-workspace\DEFAULT\EPBDS-11364_SmartRules_ExternalReturnsMatch\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6C900877-BEDA-4E1D-A8D1-D3F88AFA7983}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{167AE3FF-1EC1-4D62-B715-5BBF9D318FF6}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6465" yWindow="1215" windowWidth="15495" windowHeight="14775" xr2:uid="{446C15BB-6418-40B9-B47A-78DE9A117946}"/>
+    <workbookView xWindow="3390" yWindow="1200" windowWidth="21225" windowHeight="13500" xr2:uid="{446C15BB-6418-40B9-B47A-78DE9A117946}"/>
   </bookViews>
   <sheets>
     <sheet name="Лист1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="31">
   <si>
     <t>Conditions</t>
   </si>
@@ -90,9 +90,6 @@
     <t>Integer param1</t>
   </si>
   <si>
-    <t>contains(intArr, param1)</t>
-  </si>
-  <si>
     <t>SmartRules  Double[] SmartMytestEasy(Integer param1)</t>
   </si>
   <si>
@@ -106,16 +103,32 @@
   </si>
   <si>
     <t>SmartRules  Double[] SmartMytestEasy1(Integer param1)</t>
+  </si>
+  <si>
+    <t>contains(intArr, Param1)</t>
+  </si>
+  <si>
+    <t>SmartRules  Double[] SmartMytestEasy3(Double PARAM1)</t>
+  </si>
+  <si>
+    <t>SmartRules  Double[] SmartMytestEasy4(Integer PARAM1)</t>
+  </si>
+  <si>
+    <t>SmartRules  Double[] SmartMytestEasy5(Integer PARAM1, Integer PARAM2)</t>
+  </si>
+  <si>
+    <t>SmartRules  Double[] SmartMytestEasy5(Integer p1, Integer p2)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="0"/>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
-      <color theme="1"/>
+      <color theme="1" rgb="000000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="204"/>
@@ -168,7 +181,7 @@
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellStyleXfs>
   <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -495,16 +508,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9846E7D1-1CC3-464F-B989-F058CA19C14E}">
-  <dimension ref="D3:G35"/>
+  <dimension ref="D3:G57"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="D32" sqref="D32"/>
+    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
+      <selection activeCell="J33" sqref="J33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="5" max="5" width="39.7109375" customWidth="1"/>
-    <col min="6" max="6" width="18.7109375" customWidth="1"/>
+    <col min="5" max="5" customWidth="true" width="39.7109375" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" width="18.7109375" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="3" spans="4:7" x14ac:dyDescent="0.25">
@@ -526,7 +539,7 @@
         <v>2</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>21</v>
+        <v>26</v>
       </c>
     </row>
     <row r="6" spans="4:7" x14ac:dyDescent="0.25">
@@ -570,13 +583,13 @@
         <v>2</v>
       </c>
       <c r="E12" t="s">
+        <v>22</v>
+      </c>
+      <c r="F12" t="s">
         <v>23</v>
       </c>
-      <c r="F12" t="s">
-        <v>24</v>
-      </c>
       <c r="G12" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="13" spans="4:7" x14ac:dyDescent="0.25">
@@ -604,7 +617,7 @@
         <v>19</v>
       </c>
       <c r="G14" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="16" spans="4:7" x14ac:dyDescent="0.25">
@@ -646,7 +659,7 @@
     </row>
     <row r="25" spans="4:7" x14ac:dyDescent="0.25">
       <c r="D25" s="4" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="E25" s="4"/>
       <c r="F25" s="4"/>
@@ -694,7 +707,7 @@
     </row>
     <row r="32" spans="4:7" x14ac:dyDescent="0.25">
       <c r="D32" s="4" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="E32" s="4"/>
       <c r="F32" s="4"/>
@@ -707,7 +720,7 @@
         <v>11</v>
       </c>
       <c r="F33" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="34" spans="4:6" x14ac:dyDescent="0.25">
@@ -729,6 +742,126 @@
         <v>16</v>
       </c>
       <c r="F35" s="5" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="39" spans="4:6" x14ac:dyDescent="0.25">
+      <c r="D39" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="E39" s="4"/>
+      <c r="F39" s="4"/>
+    </row>
+    <row r="40" spans="4:6" x14ac:dyDescent="0.25">
+      <c r="D40" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="E40" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F40" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="41" spans="4:6" x14ac:dyDescent="0.25">
+      <c r="D41" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="E41" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="F41" s="5" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="42" spans="4:6" x14ac:dyDescent="0.25">
+      <c r="D42" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="E42" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="F42" s="5" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="46" spans="4:6" x14ac:dyDescent="0.25">
+      <c r="D46" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="E46" s="4"/>
+      <c r="F46" s="4"/>
+    </row>
+    <row r="47" spans="4:6" x14ac:dyDescent="0.25">
+      <c r="D47" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="E47" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F47" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="48" spans="4:6" x14ac:dyDescent="0.25">
+      <c r="D48" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="E48" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="F48" s="5" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="49" spans="4:6" x14ac:dyDescent="0.25">
+      <c r="D49" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="E49" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="F49" s="5" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="54" spans="4:6" x14ac:dyDescent="0.25">
+      <c r="D54" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="E54" s="4"/>
+      <c r="F54" s="4"/>
+    </row>
+    <row r="55" spans="4:6" x14ac:dyDescent="0.25">
+      <c r="D55" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="E55" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F55" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="56" spans="4:6" x14ac:dyDescent="0.25">
+      <c r="D56" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="E56" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="F56" s="5" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="57" spans="4:6" x14ac:dyDescent="0.25">
+      <c r="D57" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="E57" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="F57" s="5" t="s">
         <v>17</v>
       </c>
     </row>

</xml_diff>

<commit_message>
EPBDS-12991 add(CustomDatatype[][], CustomDatatype[], CustomDatatype[]) returns Object[][] instead of CustomDatatype[][]
</commit_message>
<xml_diff>
--- a/STUDIO/org.openl.rules.test/test-resources/functionality/EPBDS-11364_SmartRules_ExternalReturnsMatch.xlsx
+++ b/STUDIO/org.openl.rules.test/test-resources/functionality/EPBDS-11364_SmartRules_ExternalReturnsMatch.xlsx
@@ -1,23 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23901"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25330"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mkama\.openl\user-workspace\DEFAULT\EPBDS-11364_SmartRules_ExternalReturnsMatch\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\openl-tablets\STUDIO\org.openl.rules.test\test-resources\functionality\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{167AE3FF-1EC1-4D62-B715-5BBF9D318FF6}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{37F6A26F-3D4C-4870-9043-DA87E7255C3D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3390" yWindow="1200" windowWidth="21225" windowHeight="13500" xr2:uid="{446C15BB-6418-40B9-B47A-78DE9A117946}"/>
+    <workbookView xWindow="4440" yWindow="855" windowWidth="23430" windowHeight="12045" xr2:uid="{446C15BB-6418-40B9-B47A-78DE9A117946}"/>
   </bookViews>
   <sheets>
     <sheet name="Лист1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
-    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="30">
   <si>
     <t>Conditions</t>
   </si>
@@ -93,9 +93,6 @@
     <t>SmartRules  Double[] SmartMytestEasy(Integer param1)</t>
   </si>
   <si>
-    <t>flatten(new Double[] {outParam, actionParam}, intArr)</t>
-  </si>
-  <si>
     <t>(Double[]) flatten(new Double[] {outParam, actionParam}, intArr)</t>
   </si>
   <si>
@@ -114,21 +111,20 @@
     <t>SmartRules  Double[] SmartMytestEasy4(Integer PARAM1)</t>
   </si>
   <si>
-    <t>SmartRules  Double[] SmartMytestEasy5(Integer PARAM1, Integer PARAM2)</t>
-  </si>
-  <si>
     <t>SmartRules  Double[] SmartMytestEasy5(Integer p1, Integer p2)</t>
+  </si>
+  <si>
+    <t>(Number[]) flatten(new Double[] {outParam, actionParam}, intArr)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="0"/>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
-      <color theme="1" rgb="000000"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="204"/>
@@ -181,7 +177,7 @@
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -510,14 +506,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9846E7D1-1CC3-464F-B989-F058CA19C14E}">
   <dimension ref="D3:G57"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
-      <selection activeCell="J33" sqref="J33"/>
+    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="H17" sqref="H17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="5" max="5" customWidth="true" width="39.7109375" collapsed="true"/>
-    <col min="6" max="6" customWidth="true" width="18.7109375" collapsed="true"/>
+    <col min="5" max="5" width="39.7109375" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="18.7109375" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="3" spans="4:7" x14ac:dyDescent="0.25">
@@ -539,7 +535,7 @@
         <v>2</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="6" spans="4:7" x14ac:dyDescent="0.25">
@@ -583,13 +579,13 @@
         <v>2</v>
       </c>
       <c r="E12" t="s">
+        <v>29</v>
+      </c>
+      <c r="F12" t="s">
         <v>22</v>
       </c>
-      <c r="F12" t="s">
-        <v>23</v>
-      </c>
       <c r="G12" t="s">
-        <v>22</v>
+        <v>29</v>
       </c>
     </row>
     <row r="13" spans="4:7" x14ac:dyDescent="0.25">
@@ -617,7 +613,7 @@
         <v>19</v>
       </c>
       <c r="G14" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="16" spans="4:7" x14ac:dyDescent="0.25">
@@ -707,7 +703,7 @@
     </row>
     <row r="32" spans="4:7" x14ac:dyDescent="0.25">
       <c r="D32" s="4" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="E32" s="4"/>
       <c r="F32" s="4"/>
@@ -720,7 +716,7 @@
         <v>11</v>
       </c>
       <c r="F33" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="34" spans="4:6" x14ac:dyDescent="0.25">
@@ -747,7 +743,7 @@
     </row>
     <row r="39" spans="4:6" x14ac:dyDescent="0.25">
       <c r="D39" s="4" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="E39" s="4"/>
       <c r="F39" s="4"/>
@@ -787,7 +783,7 @@
     </row>
     <row r="46" spans="4:6" x14ac:dyDescent="0.25">
       <c r="D46" s="4" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="E46" s="4"/>
       <c r="F46" s="4"/>
@@ -827,7 +823,7 @@
     </row>
     <row r="54" spans="4:6" x14ac:dyDescent="0.25">
       <c r="D54" s="4" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="E54" s="4"/>
       <c r="F54" s="4"/>

</xml_diff>